<commit_message>
Final corrections in the dataset
</commit_message>
<xml_diff>
--- a/drinks_df.xlsx
+++ b/drinks_df.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="167">
   <si>
     <t>id</t>
   </si>
@@ -224,6 +224,75 @@
   </si>
   <si>
     <t>Spiced Wheat Beer.</t>
+  </si>
+  <si>
+    <t>09/2007</t>
+  </si>
+  <si>
+    <t>04/2008</t>
+  </si>
+  <si>
+    <t>11/2015</t>
+  </si>
+  <si>
+    <t>09/2013</t>
+  </si>
+  <si>
+    <t>02/2011</t>
+  </si>
+  <si>
+    <t>05/2013</t>
+  </si>
+  <si>
+    <t>07/2012</t>
+  </si>
+  <si>
+    <t>03/2013</t>
+  </si>
+  <si>
+    <t>03/2010</t>
+  </si>
+  <si>
+    <t>01/2011</t>
+  </si>
+  <si>
+    <t>04/2013</t>
+  </si>
+  <si>
+    <t>12/2015</t>
+  </si>
+  <si>
+    <t>11/2009</t>
+  </si>
+  <si>
+    <t>02/2010</t>
+  </si>
+  <si>
+    <t>01/2012</t>
+  </si>
+  <si>
+    <t>04/2011</t>
+  </si>
+  <si>
+    <t>08/2014</t>
+  </si>
+  <si>
+    <t>06/2013</t>
+  </si>
+  <si>
+    <t>03/2011</t>
+  </si>
+  <si>
+    <t>12/2008</t>
+  </si>
+  <si>
+    <t>12/2007</t>
+  </si>
+  <si>
+    <t>06/2011</t>
+  </si>
+  <si>
+    <t>10/2008</t>
   </si>
   <si>
     <t>A light, crisp and bitter IPA brewed with English and American hops. A small batch brewed only once.</t>
@@ -452,9 +521,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -518,12 +584,11 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -901,14 +966,14 @@
       <c r="D2" t="s">
         <v>45</v>
       </c>
-      <c r="E2" s="2">
-        <v>39326</v>
+      <c r="E2" t="s">
+        <v>70</v>
       </c>
       <c r="F2" t="s">
-        <v>70</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="H2">
         <v>4.5</v>
@@ -938,19 +1003,19 @@
         <v>20</v>
       </c>
       <c r="Q2" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="R2">
         <v>25</v>
       </c>
       <c r="S2" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="T2" t="s">
-        <v>117</v>
+        <v>140</v>
       </c>
       <c r="U2" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -966,14 +1031,14 @@
       <c r="D3" t="s">
         <v>46</v>
       </c>
-      <c r="E3" s="2">
-        <v>39539</v>
+      <c r="E3" t="s">
+        <v>71</v>
       </c>
       <c r="F3" t="s">
-        <v>71</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>119</v>
       </c>
       <c r="H3">
         <v>4.1</v>
@@ -1003,19 +1068,19 @@
         <v>20</v>
       </c>
       <c r="Q3" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="R3">
         <v>25</v>
       </c>
       <c r="S3" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="T3" t="s">
-        <v>118</v>
+        <v>141</v>
       </c>
       <c r="U3" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -1031,14 +1096,14 @@
       <c r="D4" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="2">
-        <v>42309</v>
+      <c r="E4" t="s">
+        <v>72</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
-      </c>
-      <c r="G4" s="3" t="s">
         <v>95</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="H4">
         <v>4.2</v>
@@ -1068,19 +1133,19 @@
         <v>20</v>
       </c>
       <c r="Q4" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="R4">
         <v>25</v>
       </c>
       <c r="S4" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="T4" t="s">
-        <v>119</v>
+        <v>142</v>
       </c>
       <c r="U4" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -1096,14 +1161,14 @@
       <c r="D5" t="s">
         <v>48</v>
       </c>
-      <c r="E5" s="2">
-        <v>41518</v>
+      <c r="E5" t="s">
+        <v>73</v>
       </c>
       <c r="F5" t="s">
-        <v>73</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>120</v>
       </c>
       <c r="H5">
         <v>6.3</v>
@@ -1133,19 +1198,19 @@
         <v>20</v>
       </c>
       <c r="Q5" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="R5">
         <v>25</v>
       </c>
       <c r="S5" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="T5" t="s">
-        <v>120</v>
+        <v>143</v>
       </c>
       <c r="U5" t="s">
-        <v>143</v>
+        <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -1161,14 +1226,14 @@
       <c r="D6" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="2">
-        <v>40575</v>
+      <c r="E6" t="s">
+        <v>74</v>
       </c>
       <c r="F6" t="s">
-        <v>74</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>121</v>
       </c>
       <c r="H6">
         <v>7.2</v>
@@ -1198,19 +1263,19 @@
         <v>20</v>
       </c>
       <c r="Q6" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="R6">
         <v>25</v>
       </c>
       <c r="S6" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="T6" t="s">
-        <v>121</v>
+        <v>144</v>
       </c>
       <c r="U6" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -1226,14 +1291,14 @@
       <c r="D7" t="s">
         <v>50</v>
       </c>
-      <c r="E7" s="2">
-        <v>41395</v>
+      <c r="E7" t="s">
+        <v>75</v>
       </c>
       <c r="F7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>122</v>
       </c>
       <c r="H7">
         <v>5.2</v>
@@ -1263,19 +1328,19 @@
         <v>20</v>
       </c>
       <c r="Q7" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="R7">
         <v>25</v>
       </c>
       <c r="S7" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="T7" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="U7" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -1291,14 +1356,14 @@
       <c r="D8" t="s">
         <v>51</v>
       </c>
-      <c r="E8" s="2">
-        <v>41091</v>
+      <c r="E8" t="s">
+        <v>76</v>
       </c>
       <c r="F8" t="s">
-        <v>76</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>123</v>
       </c>
       <c r="H8">
         <v>11.2</v>
@@ -1328,19 +1393,19 @@
         <v>20</v>
       </c>
       <c r="Q8" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="R8">
         <v>25</v>
       </c>
       <c r="S8" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="T8" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="U8" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -1356,14 +1421,14 @@
       <c r="D9" t="s">
         <v>52</v>
       </c>
-      <c r="E9" s="2">
-        <v>41334</v>
+      <c r="E9" t="s">
+        <v>77</v>
       </c>
       <c r="F9" t="s">
-        <v>77</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>124</v>
       </c>
       <c r="H9">
         <v>4.7</v>
@@ -1393,19 +1458,19 @@
         <v>20</v>
       </c>
       <c r="Q9" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="R9">
         <v>25</v>
       </c>
       <c r="S9" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="T9" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="U9" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -1421,14 +1486,14 @@
       <c r="D10" t="s">
         <v>53</v>
       </c>
-      <c r="E10" s="2">
-        <v>40238</v>
+      <c r="E10" t="s">
+        <v>78</v>
       </c>
       <c r="F10" t="s">
-        <v>78</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="H10">
         <v>12.5</v>
@@ -1458,19 +1523,19 @@
         <v>20</v>
       </c>
       <c r="Q10" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="R10">
         <v>25</v>
       </c>
       <c r="S10" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="T10" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="U10" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -1486,14 +1551,14 @@
       <c r="D11" t="s">
         <v>54</v>
       </c>
-      <c r="E11" s="2">
-        <v>40544</v>
+      <c r="E11" t="s">
+        <v>79</v>
       </c>
       <c r="F11" t="s">
-        <v>79</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>126</v>
       </c>
       <c r="H11">
         <v>7.5</v>
@@ -1523,19 +1588,19 @@
         <v>20</v>
       </c>
       <c r="Q11" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="R11">
         <v>25</v>
       </c>
       <c r="S11" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="T11" t="s">
-        <v>126</v>
+        <v>149</v>
       </c>
       <c r="U11" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -1551,14 +1616,14 @@
       <c r="D12" t="s">
         <v>55</v>
       </c>
-      <c r="E12" s="2">
-        <v>41365</v>
+      <c r="E12" t="s">
+        <v>80</v>
       </c>
       <c r="F12" t="s">
-        <v>80</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>95</v>
+        <v>103</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="H12">
         <v>7.3</v>
@@ -1588,19 +1653,19 @@
         <v>20</v>
       </c>
       <c r="Q12" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="R12">
         <v>25</v>
       </c>
       <c r="S12" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="T12" t="s">
-        <v>127</v>
+        <v>150</v>
       </c>
       <c r="U12" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -1616,14 +1681,14 @@
       <c r="D13" t="s">
         <v>56</v>
       </c>
-      <c r="E13" s="2">
-        <v>42339</v>
+      <c r="E13" t="s">
+        <v>81</v>
       </c>
       <c r="F13" t="s">
-        <v>81</v>
-      </c>
-      <c r="G13" s="3" t="s">
         <v>104</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="H13">
         <v>5.3</v>
@@ -1653,19 +1718,19 @@
         <v>20</v>
       </c>
       <c r="Q13" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="R13">
         <v>25</v>
       </c>
       <c r="S13" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="T13" t="s">
-        <v>128</v>
+        <v>151</v>
       </c>
       <c r="U13" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -1681,14 +1746,14 @@
       <c r="D14" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="2">
-        <v>40118</v>
+      <c r="E14" t="s">
+        <v>82</v>
       </c>
       <c r="F14" t="s">
-        <v>82</v>
-      </c>
-      <c r="G14" s="3" t="s">
         <v>105</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>128</v>
       </c>
       <c r="H14">
         <v>4.5</v>
@@ -1718,19 +1783,19 @@
         <v>20</v>
       </c>
       <c r="Q14" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="R14">
         <v>25</v>
       </c>
       <c r="S14" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="T14" t="s">
-        <v>129</v>
+        <v>152</v>
       </c>
       <c r="U14" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -1746,14 +1811,14 @@
       <c r="D15" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="2">
-        <v>40210</v>
+      <c r="E15" t="s">
+        <v>83</v>
       </c>
       <c r="F15" t="s">
-        <v>83</v>
-      </c>
-      <c r="G15" s="3" t="s">
         <v>106</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>129</v>
       </c>
       <c r="H15">
         <v>4.5</v>
@@ -1783,19 +1848,19 @@
         <v>20</v>
       </c>
       <c r="Q15" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="R15">
         <v>25</v>
       </c>
       <c r="S15" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="T15" t="s">
-        <v>130</v>
+        <v>153</v>
       </c>
       <c r="U15" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -1811,14 +1876,14 @@
       <c r="D16" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="2">
-        <v>40909</v>
+      <c r="E16" t="s">
+        <v>84</v>
       </c>
       <c r="F16" t="s">
-        <v>84</v>
-      </c>
-      <c r="G16" s="3" t="s">
         <v>107</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>130</v>
       </c>
       <c r="H16">
         <v>14.5</v>
@@ -1848,19 +1913,19 @@
         <v>20</v>
       </c>
       <c r="Q16" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="R16">
         <v>25</v>
       </c>
       <c r="S16" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="T16" t="s">
-        <v>131</v>
+        <v>154</v>
       </c>
       <c r="U16" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -1876,14 +1941,14 @@
       <c r="D17" t="s">
         <v>60</v>
       </c>
-      <c r="E17" s="2">
-        <v>40909</v>
+      <c r="E17" t="s">
+        <v>84</v>
       </c>
       <c r="F17" t="s">
-        <v>85</v>
-      </c>
-      <c r="G17" s="3" t="s">
         <v>108</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>131</v>
       </c>
       <c r="H17">
         <v>6.1</v>
@@ -1913,19 +1978,19 @@
         <v>20</v>
       </c>
       <c r="Q17" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="R17">
         <v>25</v>
       </c>
       <c r="S17" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="T17" t="s">
-        <v>132</v>
+        <v>155</v>
       </c>
       <c r="U17" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
     </row>
     <row r="18" spans="1:21">
@@ -1941,14 +2006,14 @@
       <c r="D18" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="2">
-        <v>40634</v>
+      <c r="E18" t="s">
+        <v>85</v>
       </c>
       <c r="F18" t="s">
-        <v>86</v>
-      </c>
-      <c r="G18" s="3" t="s">
         <v>109</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>132</v>
       </c>
       <c r="H18">
         <v>11.2</v>
@@ -1968,9 +2033,6 @@
       <c r="M18">
         <v>35</v>
       </c>
-      <c r="N18">
-        <v>0</v>
-      </c>
       <c r="O18">
         <v>87</v>
       </c>
@@ -1978,19 +2040,19 @@
         <v>20</v>
       </c>
       <c r="Q18" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="R18">
         <v>25</v>
       </c>
       <c r="S18" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="T18" t="s">
-        <v>133</v>
+        <v>156</v>
       </c>
       <c r="U18" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
     </row>
     <row r="19" spans="1:21">
@@ -2006,14 +2068,14 @@
       <c r="D19" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="2">
-        <v>41852</v>
+      <c r="E19" t="s">
+        <v>86</v>
       </c>
       <c r="F19" t="s">
-        <v>87</v>
-      </c>
-      <c r="G19" s="3" t="s">
         <v>110</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>133</v>
       </c>
       <c r="H19">
         <v>6</v>
@@ -2043,19 +2105,19 @@
         <v>20</v>
       </c>
       <c r="Q19" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="R19">
         <v>25</v>
       </c>
       <c r="S19" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="T19" t="s">
-        <v>134</v>
+        <v>157</v>
       </c>
       <c r="U19" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
     </row>
     <row r="20" spans="1:21">
@@ -2071,14 +2133,14 @@
       <c r="D20" t="s">
         <v>63</v>
       </c>
-      <c r="E20" s="2">
-        <v>41426</v>
+      <c r="E20" t="s">
+        <v>87</v>
       </c>
       <c r="F20" t="s">
-        <v>88</v>
-      </c>
-      <c r="G20" s="3" t="s">
         <v>111</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>134</v>
       </c>
       <c r="H20">
         <v>8.199999999999999</v>
@@ -2092,12 +2154,6 @@
       <c r="K20">
         <v>1076</v>
       </c>
-      <c r="L20">
-        <v>0</v>
-      </c>
-      <c r="M20">
-        <v>0</v>
-      </c>
       <c r="N20">
         <v>4.4</v>
       </c>
@@ -2108,19 +2164,19 @@
         <v>20</v>
       </c>
       <c r="Q20" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="R20">
         <v>25</v>
       </c>
       <c r="S20" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="T20" t="s">
-        <v>135</v>
+        <v>158</v>
       </c>
       <c r="U20" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
     </row>
     <row r="21" spans="1:21">
@@ -2136,14 +2192,14 @@
       <c r="D21" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="2">
-        <v>40603</v>
+      <c r="E21" t="s">
+        <v>88</v>
       </c>
       <c r="F21" t="s">
-        <v>89</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>95</v>
+        <v>112</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="H21">
         <v>10.27</v>
@@ -2173,19 +2229,19 @@
         <v>20</v>
       </c>
       <c r="Q21" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="R21">
         <v>25</v>
       </c>
       <c r="S21" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="T21" t="s">
-        <v>136</v>
+        <v>159</v>
       </c>
       <c r="U21" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
     </row>
     <row r="22" spans="1:21">
@@ -2201,14 +2257,14 @@
       <c r="D22" t="s">
         <v>65</v>
       </c>
-      <c r="E22" s="2">
-        <v>41365</v>
+      <c r="E22" t="s">
+        <v>80</v>
       </c>
       <c r="F22" t="s">
-        <v>90</v>
-      </c>
-      <c r="G22" s="3" t="s">
-        <v>95</v>
+        <v>113</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>118</v>
       </c>
       <c r="H22">
         <v>4.3</v>
@@ -2238,19 +2294,19 @@
         <v>20</v>
       </c>
       <c r="Q22" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="R22">
         <v>25</v>
       </c>
       <c r="S22" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="T22" t="s">
-        <v>137</v>
+        <v>160</v>
       </c>
       <c r="U22" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
     </row>
     <row r="23" spans="1:21">
@@ -2266,14 +2322,14 @@
       <c r="D23" t="s">
         <v>66</v>
       </c>
-      <c r="E23" s="2">
-        <v>39783</v>
+      <c r="E23" t="s">
+        <v>89</v>
       </c>
       <c r="F23" t="s">
-        <v>91</v>
-      </c>
-      <c r="G23" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>135</v>
       </c>
       <c r="H23">
         <v>12.5</v>
@@ -2303,19 +2359,19 @@
         <v>20</v>
       </c>
       <c r="Q23" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="R23">
         <v>25</v>
       </c>
       <c r="S23" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="T23" t="s">
-        <v>138</v>
+        <v>161</v>
       </c>
       <c r="U23" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
     </row>
     <row r="24" spans="1:21">
@@ -2331,14 +2387,14 @@
       <c r="D24" t="s">
         <v>67</v>
       </c>
-      <c r="E24" s="2">
-        <v>39417</v>
+      <c r="E24" t="s">
+        <v>90</v>
       </c>
       <c r="F24" t="s">
-        <v>92</v>
-      </c>
-      <c r="G24" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>136</v>
       </c>
       <c r="H24">
         <v>8</v>
@@ -2368,19 +2424,19 @@
         <v>20</v>
       </c>
       <c r="Q24" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="R24">
         <v>25</v>
       </c>
       <c r="S24" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="T24" t="s">
-        <v>139</v>
+        <v>162</v>
       </c>
       <c r="U24" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
     </row>
     <row r="25" spans="1:21">
@@ -2396,33 +2452,24 @@
       <c r="D25" t="s">
         <v>68</v>
       </c>
-      <c r="E25" s="2">
-        <v>40695</v>
+      <c r="E25" t="s">
+        <v>91</v>
       </c>
       <c r="F25" t="s">
-        <v>93</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>137</v>
       </c>
       <c r="H25">
         <v>55</v>
       </c>
-      <c r="I25">
-        <v>0</v>
-      </c>
       <c r="J25">
         <v>1000</v>
       </c>
       <c r="K25">
         <v>1112</v>
       </c>
-      <c r="L25">
-        <v>0</v>
-      </c>
-      <c r="M25">
-        <v>0</v>
-      </c>
       <c r="N25">
         <v>4.4</v>
       </c>
@@ -2433,19 +2480,19 @@
         <v>20</v>
       </c>
       <c r="Q25" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="R25">
         <v>25</v>
       </c>
       <c r="S25" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="T25" t="s">
-        <v>140</v>
+        <v>163</v>
       </c>
       <c r="U25" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" spans="1:21">
@@ -2461,14 +2508,14 @@
       <c r="D26" t="s">
         <v>69</v>
       </c>
-      <c r="E26" s="2">
-        <v>39722</v>
+      <c r="E26" t="s">
+        <v>92</v>
       </c>
       <c r="F26" t="s">
-        <v>94</v>
-      </c>
-      <c r="G26" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>138</v>
       </c>
       <c r="H26">
         <v>4.7</v>
@@ -2498,19 +2545,19 @@
         <v>20</v>
       </c>
       <c r="Q26" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="R26">
         <v>25</v>
       </c>
       <c r="S26" t="s">
-        <v>116</v>
+        <v>139</v>
       </c>
       <c r="T26" t="s">
-        <v>141</v>
+        <v>164</v>
       </c>
       <c r="U26" t="s">
-        <v>142</v>
+        <v>165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>